<commit_message>
changes to audio load speed
</commit_message>
<xml_diff>
--- a/lexicon backup.xlsx
+++ b/lexicon backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjohns/Desktop/Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F666E37E-56D1-314B-9802-90E17E19437C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82F0940-9674-9F45-A1F6-50CE0D48CD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="660" windowWidth="13000" windowHeight="20520" xr2:uid="{94D6E9CA-AF84-3445-BCA6-352956A682AC}"/>
   </bookViews>
@@ -3527,9 +3527,6 @@
     <t>audio/examples/thishardthinginourheadisaskull.mp3</t>
   </si>
   <si>
-    <t>audio/examples/haveyouheverseenamountainlion.mp3</t>
-  </si>
-  <si>
     <t>audio/examples/thebobcatsarefriendly.mp3</t>
   </si>
   <si>
@@ -3558,6 +3555,9 @@
   </si>
   <si>
     <t>audio/examples/hangupthesaddle.mp3</t>
+  </si>
+  <si>
+    <t>audio/examples/haveyoueverseenamountainlion.mp3</t>
   </si>
 </sst>
 </file>
@@ -3944,10 +3944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C70B7F-39B1-CF49-AFC9-B05A2423C135}">
-  <dimension ref="A1:N139"/>
+  <dimension ref="A1:O139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K92" zoomScale="113" workbookViewId="0">
-      <selection activeCell="N98" sqref="N98"/>
+    <sheetView tabSelected="1" topLeftCell="L84" zoomScale="113" workbookViewId="0">
+      <selection activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7170,7 +7170,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>674</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>679</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>684</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>693</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>701</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>709</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>717</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>725</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>730</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>739</v>
       </c>
@@ -7532,10 +7532,10 @@
         <v>747</v>
       </c>
       <c r="N90" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>748</v>
       </c>
@@ -7573,10 +7573,10 @@
         <v>756</v>
       </c>
       <c r="N91" t="s">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>757</v>
       </c>
@@ -7614,10 +7614,13 @@
         <v>764</v>
       </c>
       <c r="N92" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>1164</v>
+      </c>
+      <c r="O92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>765</v>
       </c>
@@ -7655,10 +7658,10 @@
         <v>773</v>
       </c>
       <c r="N93" t="s">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>774</v>
       </c>
@@ -7696,10 +7699,10 @@
         <v>782</v>
       </c>
       <c r="N94" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>783</v>
       </c>
@@ -7737,10 +7740,10 @@
         <v>790</v>
       </c>
       <c r="N95" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>791</v>
       </c>
@@ -7778,7 +7781,7 @@
         <v>799</v>
       </c>
       <c r="N96" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7819,7 +7822,7 @@
         <v>808</v>
       </c>
       <c r="N97" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -7984,7 +7987,7 @@
         <v>841</v>
       </c>
       <c r="N103" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -8019,7 +8022,7 @@
         <v>847</v>
       </c>
       <c r="N104" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -8100,7 +8103,7 @@
         <v>864</v>
       </c>
       <c r="N107" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to search feature
</commit_message>
<xml_diff>
--- a/lexicon backup.xlsx
+++ b/lexicon backup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjohns/Desktop/Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82F0940-9674-9F45-A1F6-50CE0D48CD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16B6E3F-9A9A-D84D-9BBB-7568DEC4DA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="660" windowWidth="13000" windowHeight="20520" xr2:uid="{94D6E9CA-AF84-3445-BCA6-352956A682AC}"/>
+    <workbookView xWindow="900" yWindow="660" windowWidth="28400" windowHeight="20520" xr2:uid="{94D6E9CA-AF84-3445-BCA6-352956A682AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="1189">
   <si>
     <t>oodham</t>
   </si>
@@ -3179,9 +3179,6 @@
     <t>[ˈhɔ.hɑ]</t>
   </si>
   <si>
-    <t>Tohono O'odham</t>
-  </si>
-  <si>
     <t>cup</t>
   </si>
   <si>
@@ -3558,6 +3555,54 @@
   </si>
   <si>
     <t>audio/examples/haveyoueverseenamountainlion.mp3</t>
+  </si>
+  <si>
+    <t>ceoj</t>
+  </si>
+  <si>
+    <t>man, male</t>
+  </si>
+  <si>
+    <t>[cɯɔɟ̥]</t>
+  </si>
+  <si>
+    <t>cecoj</t>
+  </si>
+  <si>
+    <t>[ˈcɯ.cɔɟ̥]</t>
+  </si>
+  <si>
+    <t>men, males</t>
+  </si>
+  <si>
+    <t>’uvĭ</t>
+  </si>
+  <si>
+    <t>woman, female</t>
+  </si>
+  <si>
+    <t>[ˈʔu.vĭ]</t>
+  </si>
+  <si>
+    <t>’u’uvĭ</t>
+  </si>
+  <si>
+    <t>[ˈʔu.ʔu.vĭ]</t>
+  </si>
+  <si>
+    <t>women, females</t>
+  </si>
+  <si>
+    <t>’O’odham</t>
+  </si>
+  <si>
+    <t>person, O’odham person // people, O’odham people</t>
+  </si>
+  <si>
+    <t>[ˈʔɔ.ʔɔd.hɑm]</t>
+  </si>
+  <si>
+    <t>Any||Tohono O'odham</t>
   </si>
 </sst>
 </file>
@@ -3944,10 +3989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C70B7F-39B1-CF49-AFC9-B05A2423C135}">
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L84" zoomScale="113" workbookViewId="0">
-      <selection activeCell="Q92" sqref="Q92"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4049,7 +4094,7 @@
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -4093,7 +4138,7 @@
         <v>1036</v>
       </c>
       <c r="N3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -4134,7 +4179,7 @@
         <v>40</v>
       </c>
       <c r="N4" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -4175,7 +4220,7 @@
         <v>49</v>
       </c>
       <c r="N5" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -4216,7 +4261,7 @@
         <v>58</v>
       </c>
       <c r="N6" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -4257,7 +4302,7 @@
         <v>67</v>
       </c>
       <c r="N7" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -4298,7 +4343,7 @@
         <v>76</v>
       </c>
       <c r="N8" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4339,7 +4384,7 @@
         <v>85</v>
       </c>
       <c r="N9" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4380,7 +4425,7 @@
         <v>89</v>
       </c>
       <c r="N10" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4421,7 +4466,7 @@
         <v>97</v>
       </c>
       <c r="N11" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4462,7 +4507,7 @@
         <v>106</v>
       </c>
       <c r="N12" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -4503,7 +4548,7 @@
         <v>115</v>
       </c>
       <c r="N13" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -4544,7 +4589,7 @@
         <v>124</v>
       </c>
       <c r="N14" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -4585,7 +4630,7 @@
         <v>133</v>
       </c>
       <c r="N15" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -4626,7 +4671,7 @@
         <v>142</v>
       </c>
       <c r="N16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -4667,7 +4712,7 @@
         <v>151</v>
       </c>
       <c r="N17" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4693,7 +4738,7 @@
         <v>156</v>
       </c>
       <c r="N18" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="136" x14ac:dyDescent="0.2">
@@ -4734,7 +4779,7 @@
         <v>165</v>
       </c>
       <c r="N19" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -4763,7 +4808,7 @@
         <v>171</v>
       </c>
       <c r="N20" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4804,7 +4849,7 @@
         <v>180</v>
       </c>
       <c r="N21" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -4845,7 +4890,7 @@
         <v>189</v>
       </c>
       <c r="N22" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -4886,7 +4931,7 @@
         <v>198</v>
       </c>
       <c r="N23" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -4927,7 +4972,7 @@
         <v>207</v>
       </c>
       <c r="N24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4968,7 +5013,7 @@
         <v>216</v>
       </c>
       <c r="N25" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -4997,7 +5042,7 @@
         <v>223</v>
       </c>
       <c r="N26" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5038,7 +5083,7 @@
         <v>232</v>
       </c>
       <c r="N27" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -5070,7 +5115,7 @@
         <v>1043</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="K28" t="s">
         <v>239</v>
@@ -5079,7 +5124,7 @@
         <v>240</v>
       </c>
       <c r="N28" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -5120,7 +5165,7 @@
         <v>249</v>
       </c>
       <c r="N29" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -5161,7 +5206,7 @@
         <v>258</v>
       </c>
       <c r="N30" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5193,7 +5238,7 @@
         <v>1043</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="K31" t="s">
         <v>265</v>
@@ -5202,7 +5247,7 @@
         <v>266</v>
       </c>
       <c r="N31" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5243,7 +5288,7 @@
         <v>275</v>
       </c>
       <c r="N32" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5284,7 +5329,7 @@
         <v>291</v>
       </c>
       <c r="N33" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5325,7 +5370,7 @@
         <v>284</v>
       </c>
       <c r="N34" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -5366,7 +5411,7 @@
         <v>298</v>
       </c>
       <c r="N35" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5407,7 +5452,7 @@
         <v>307</v>
       </c>
       <c r="N36" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5448,7 +5493,7 @@
         <v>316</v>
       </c>
       <c r="N37" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5480,7 +5525,7 @@
         <v>1043</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="K38" t="s">
         <v>323</v>
@@ -5489,7 +5534,7 @@
         <v>324</v>
       </c>
       <c r="N38" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5530,7 +5575,7 @@
         <v>333</v>
       </c>
       <c r="N39" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -5571,7 +5616,7 @@
         <v>342</v>
       </c>
       <c r="N40" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5612,7 +5657,7 @@
         <v>349</v>
       </c>
       <c r="N41" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5653,7 +5698,7 @@
         <v>358</v>
       </c>
       <c r="N42" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -5694,7 +5739,7 @@
         <v>367</v>
       </c>
       <c r="N43" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -5735,7 +5780,7 @@
         <v>375</v>
       </c>
       <c r="N44" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5776,7 +5821,7 @@
         <v>384</v>
       </c>
       <c r="N45" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5817,7 +5862,7 @@
         <v>393</v>
       </c>
       <c r="N46" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -5858,7 +5903,7 @@
         <v>402</v>
       </c>
       <c r="N47" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5899,7 +5944,7 @@
         <v>411</v>
       </c>
       <c r="N48" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -5940,7 +5985,7 @@
         <v>420</v>
       </c>
       <c r="N49" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -5981,7 +6026,7 @@
         <v>429</v>
       </c>
       <c r="N50" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6022,7 +6067,7 @@
         <v>438</v>
       </c>
       <c r="N51" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6063,7 +6108,7 @@
         <v>447</v>
       </c>
       <c r="N52" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6104,7 +6149,7 @@
         <v>456</v>
       </c>
       <c r="N53" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6145,7 +6190,7 @@
         <v>463</v>
       </c>
       <c r="N54" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6186,7 +6231,7 @@
         <v>472</v>
       </c>
       <c r="N55" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6218,7 +6263,7 @@
         <v>1043</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="K56" t="s">
         <v>479</v>
@@ -6227,7 +6272,7 @@
         <v>480</v>
       </c>
       <c r="N56" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6268,7 +6313,7 @@
         <v>489</v>
       </c>
       <c r="N57" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6309,7 +6354,7 @@
         <v>498</v>
       </c>
       <c r="N58" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6341,7 +6386,7 @@
         <v>1043</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="K59" t="s">
         <v>505</v>
@@ -6350,7 +6395,7 @@
         <v>506</v>
       </c>
       <c r="N59" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6382,7 +6427,7 @@
         <v>1043</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K60" t="s">
         <v>513</v>
@@ -6391,7 +6436,7 @@
         <v>514</v>
       </c>
       <c r="N60" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6432,7 +6477,7 @@
         <v>523</v>
       </c>
       <c r="N61" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6473,7 +6518,7 @@
         <v>532</v>
       </c>
       <c r="N62" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6514,7 +6559,7 @@
         <v>541</v>
       </c>
       <c r="N63" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -6546,7 +6591,7 @@
         <v>1043</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="K64" t="s">
         <v>548</v>
@@ -6555,7 +6600,7 @@
         <v>549</v>
       </c>
       <c r="N64" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6596,7 +6641,7 @@
         <v>558</v>
       </c>
       <c r="N65" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6637,7 +6682,7 @@
         <v>567</v>
       </c>
       <c r="N66" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6663,7 +6708,7 @@
         <v>572</v>
       </c>
       <c r="N67" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6704,7 +6749,7 @@
         <v>581</v>
       </c>
       <c r="N68" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6745,7 +6790,7 @@
         <v>590</v>
       </c>
       <c r="N69" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6786,7 +6831,7 @@
         <v>599</v>
       </c>
       <c r="N70" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6827,7 +6872,7 @@
         <v>608</v>
       </c>
       <c r="N71" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6857,7 +6902,7 @@
         <v>613</v>
       </c>
       <c r="N72" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="85" x14ac:dyDescent="0.2">
@@ -6877,13 +6922,13 @@
         <v>1043</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="K73" t="s">
         <v>617</v>
       </c>
       <c r="N73" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6924,7 +6969,7 @@
         <v>626</v>
       </c>
       <c r="N74" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6965,7 +7010,7 @@
         <v>635</v>
       </c>
       <c r="N75" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6997,7 +7042,7 @@
         <v>1043</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="K76" t="s">
         <v>642</v>
@@ -7006,7 +7051,7 @@
         <v>643</v>
       </c>
       <c r="N76" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7047,7 +7092,7 @@
         <v>651</v>
       </c>
       <c r="N77" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7088,7 +7133,7 @@
         <v>659</v>
       </c>
       <c r="N78" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7129,7 +7174,7 @@
         <v>667</v>
       </c>
       <c r="N79" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7161,13 +7206,13 @@
         <v>1043</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="K80" t="s">
         <v>673</v>
       </c>
       <c r="N80" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7193,7 +7238,7 @@
         <v>678</v>
       </c>
       <c r="N81" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7219,7 +7264,7 @@
         <v>683</v>
       </c>
       <c r="N82" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -7260,7 +7305,7 @@
         <v>692</v>
       </c>
       <c r="N83" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7292,7 +7337,7 @@
         <v>1043</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="K84" t="s">
         <v>699</v>
@@ -7301,7 +7346,7 @@
         <v>700</v>
       </c>
       <c r="N84" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7333,7 +7378,7 @@
         <v>1043</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="K85" t="s">
         <v>707</v>
@@ -7342,7 +7387,7 @@
         <v>708</v>
       </c>
       <c r="N85" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7374,7 +7419,7 @@
         <v>1043</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="K86" t="s">
         <v>715</v>
@@ -7383,7 +7428,7 @@
         <v>716</v>
       </c>
       <c r="N86" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7415,7 +7460,7 @@
         <v>1043</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="K87" t="s">
         <v>723</v>
@@ -7424,7 +7469,7 @@
         <v>724</v>
       </c>
       <c r="N87" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7450,7 +7495,7 @@
         <v>729</v>
       </c>
       <c r="N88" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -7491,7 +7536,7 @@
         <v>738</v>
       </c>
       <c r="N89" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7532,7 +7577,7 @@
         <v>747</v>
       </c>
       <c r="N90" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -7573,7 +7618,7 @@
         <v>756</v>
       </c>
       <c r="N91" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -7605,7 +7650,7 @@
         <v>1043</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="K92" t="s">
         <v>763</v>
@@ -7614,7 +7659,7 @@
         <v>764</v>
       </c>
       <c r="N92" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="O92">
         <v>4</v>
@@ -7658,7 +7703,7 @@
         <v>773</v>
       </c>
       <c r="N93" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -7699,7 +7744,7 @@
         <v>782</v>
       </c>
       <c r="N94" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7731,7 +7776,7 @@
         <v>1043</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="K95" t="s">
         <v>789</v>
@@ -7740,7 +7785,7 @@
         <v>790</v>
       </c>
       <c r="N95" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -7781,7 +7826,7 @@
         <v>799</v>
       </c>
       <c r="N96" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7822,7 +7867,7 @@
         <v>808</v>
       </c>
       <c r="N97" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -7987,7 +8032,7 @@
         <v>841</v>
       </c>
       <c r="N103" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -8022,7 +8067,7 @@
         <v>847</v>
       </c>
       <c r="N104" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -8103,7 +8148,7 @@
         <v>864</v>
       </c>
       <c r="N107" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -8970,15 +9015,15 @@
         <v>29</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>1047</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B138" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C138" t="s">
         <v>16</v>
@@ -8987,16 +9032,16 @@
         <v>4</v>
       </c>
       <c r="E138" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F138" t="s">
         <v>1050</v>
       </c>
-      <c r="F138" t="s">
+      <c r="G138" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H138" t="s">
         <v>1051</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>1058</v>
-      </c>
-      <c r="H138" t="s">
-        <v>1052</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>1043</v>
@@ -9004,10 +9049,10 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B139" t="s">
         <v>1053</v>
-      </c>
-      <c r="B139" t="s">
-        <v>1054</v>
       </c>
       <c r="C139" t="s">
         <v>16</v>
@@ -9016,18 +9061,90 @@
         <v>2</v>
       </c>
       <c r="E139" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F139" t="s">
         <v>1055</v>
       </c>
-      <c r="F139" t="s">
+      <c r="G139" s="3" t="s">
         <v>1056</v>
       </c>
-      <c r="G139" s="3" t="s">
-        <v>1057</v>
-      </c>
       <c r="H139" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="I139" s="3" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C140" t="s">
+        <v>16</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F140" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="H140" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A141" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C141" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F141" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1184</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I142" s="3" t="s">
         <v>1043</v>
       </c>
     </row>

</xml_diff>